<commit_message>
melhorias de qualidade de vida
</commit_message>
<xml_diff>
--- a/nomes.xlsx
+++ b/nomes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo\Documents\RenoeacaoPDFs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo\Documents\RenomeacaoPDFs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2108DBAE-F931-4351-95F6-FB12BB11CA29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E28F3A1-3A8D-4200-8B21-DCB94158065F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6060" yWindow="4365" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,9 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -34,7 +37,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -48,16 +51,27 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF434343"/>
+      <name val="Lexend"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -65,17 +79,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -357,21 +407,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="52" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="27.75" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" ht="28.5" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" thickBot="1">
+      <c r="A2" s="3"/>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" thickBot="1">
+      <c r="A3" s="4"/>
+    </row>
+    <row r="4" spans="1:1" ht="15.75" thickBot="1">
+      <c r="A4" s="4"/>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5"/>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6"/>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7"/>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8"/>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>